<commit_message>
Adding axis labels to standard deviation graph.
</commit_message>
<xml_diff>
--- a/Standard Minority Game/standard-deviation-vs-memory-size.xlsx
+++ b/Standard Minority Game/standard-deviation-vs-memory-size.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="-420" windowWidth="24320" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="225" yWindow="-420" windowWidth="21720" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sigma" sheetId="2" r:id="rId1"/>
@@ -65,11 +65,20 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -93,1444 +102,1444 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="280">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="281">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="282">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="283">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="284">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="285">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="286">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="287">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="288">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="289">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="290">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="291">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="294">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="295">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="296">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="298">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="299">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="300">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="301">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="302">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="303">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="304">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="305">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="306">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="307">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="308">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="309">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="310">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="311">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="312">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="313">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="314">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="315">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="316">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="317">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="318">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="319">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="320">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="321">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="322">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="323">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="324">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="326">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="327">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="328">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="329">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="330">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="331">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="332">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="333">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="334">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="335">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="336">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="337">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="338">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="339">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="340">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="341">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="342">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="343">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="344">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="345">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="346">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="347">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="348">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="349">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="350">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="351">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="352">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="353">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="354">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="355">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="356">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="357">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="358">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="359">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="360">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="361">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="362">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="363">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="364">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="365">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="366">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="367">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="368">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="369">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="370">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="371">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="372">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="373">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="374">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="375">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="376">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="377">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="378">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="379">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="380">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="381">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="382">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="383">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="384">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="385">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="386">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="387">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="388">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="389">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="390">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="391">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="392">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="393">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="394">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="395">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="396">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="397">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="398">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="399">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="400">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="401">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="402">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="403">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="404">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="405">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="406">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="407">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="408">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="409">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="410">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="411">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="412">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="413">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="414">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="415">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="416">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="417">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="418">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="419">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="420">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="421">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="422">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="423">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="424">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="425">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="426">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="427">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="428">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="429">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="430">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="431">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="432">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="433">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="434">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="435">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="436">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="437">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="438">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="439">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="440">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="441">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="442">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="443">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="444">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="445">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="446">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="447">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="448">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="449">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="450">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="451">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="452">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="453">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="454">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="455">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="456">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="457">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="458">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="459">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="460">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="461">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="462">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="463">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="464">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="465">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="466">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="467">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="468">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="469">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="470">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="471">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="472">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="473">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="474">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="475">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="476">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="477">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="478">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="479">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,49 +1551,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
                 <c:pt idx="0">
-                  <c:v>13.5277492584686</c:v>
+                  <c:v>13.527749258468599</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13.1909059582729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.3790881602596</c:v>
+                  <c:v>13.379088160259601</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13.1529464379659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.2287565553229</c:v>
+                  <c:v>13.228756555322899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.4536240470737</c:v>
+                  <c:v>13.453624047073699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.2287565553229</c:v>
+                  <c:v>13.228756555322899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.2287565553229</c:v>
+                  <c:v>13.228756555322899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.30413469565</c:v>
+                  <c:v>13.304134695649999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.2287565553229</c:v>
+                  <c:v>13.228756555322899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.5277492584686</c:v>
+                  <c:v>13.527749258468599</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.0384048104052</c:v>
+                  <c:v>13.038404810405201</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.490737563232</c:v>
+                  <c:v>13.490737563232001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.2664991614216</c:v>
+                  <c:v>13.266499161421599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.3790881602596</c:v>
+                  <c:v>13.379088160259601</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>13.6014705087354</c:v>
@@ -1593,16 +1602,16 @@
                   <c:v>13.856406460551</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.5277492584686</c:v>
+                  <c:v>13.527749258468599</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.2287565553229</c:v>
+                  <c:v>13.228756555322899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.30413469565</c:v>
+                  <c:v>13.304134695649999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.5646599662505</c:v>
+                  <c:v>13.564659966250501</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>13.1529464379659</c:v>
@@ -1611,31 +1620,31 @@
                   <c:v>13.3416640641263</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.9614813968157</c:v>
+                  <c:v>12.961481396815699</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.3790881602596</c:v>
+                  <c:v>13.379088160259601</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.0384048104052</c:v>
+                  <c:v>13.038404810405201</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>13.1529464379659</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.4536240470737</c:v>
+                  <c:v>13.453624047073699</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.2664991614216</c:v>
+                  <c:v>13.266499161421599</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>13.7840487520902</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.30413469565</c:v>
+                  <c:v>13.304134695649999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.114877048604</c:v>
+                  <c:v>13.114877048604001</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>12.1243556529821</c:v>
@@ -1647,16 +1656,16 @@
                   <c:v>11.8321595661992</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.9582607431013</c:v>
+                  <c:v>11.958260743101301</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.7046999107196</c:v>
+                  <c:v>11.704699910719601</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>11.6619037896906</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12.3288280059379</c:v>
+                  <c:v>12.328828005937901</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>12.5299640861416</c:v>
@@ -1665,7 +1674,7 @@
                   <c:v>11.6619037896906</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.5758369027902</c:v>
+                  <c:v>11.575836902790201</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>12.5698050899765</c:v>
@@ -1680,19 +1689,19 @@
                   <c:v>11.7473401244707</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.3578166916005</c:v>
+                  <c:v>11.357816691600499</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.5325625946707</c:v>
+                  <c:v>11.532562594670701</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>11.4455231422595</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.9163752878129</c:v>
+                  <c:v>11.916375287812899</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>11.9163752878129</c:v>
+                  <c:v>11.916375287812899</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>11.6619037896906</c:v>
@@ -1701,16 +1710,16 @@
                   <c:v>11.6619037896906</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12.3693168768529</c:v>
+                  <c:v>12.369316876852899</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>12.0415945787922</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>11.8743420870379</c:v>
+                  <c:v>11.874342087037901</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>12.3693168768529</c:v>
+                  <c:v>12.369316876852899</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>12.1243556529821</c:v>
@@ -1719,10 +1728,10 @@
                   <c:v>12.0415945787922</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>11.5325625946707</c:v>
+                  <c:v>11.532562594670701</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>11.7898261225515</c:v>
+                  <c:v>11.789826122551499</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>11.6619037896906</c:v>
@@ -1731,1288 +1740,1354 @@
                   <c:v>11.13552872566</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>12.4899959967967</c:v>
+                  <c:v>12.489995996796701</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791442992</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791442992</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>9.32737905308881</c:v>
+                  <c:v>9.3273790530888103</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>7.28010988928051</c:v>
+                  <c:v>7.2801098892805101</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>7.28010988928051</c:v>
+                  <c:v>7.2801098892805101</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>7.07106781186547</c:v>
+                  <c:v>7.0710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>6.48074069840786</c:v>
+                  <c:v>6.4807406984078604</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>5.91607978309961</c:v>
+                  <c:v>5.9160797830996108</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>6.40312423743284</c:v>
+                  <c:v>6.4031242374328396</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>5.8309518948453</c:v>
+                  <c:v>5.8309518948452999</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>6.24499799839839</c:v>
+                  <c:v>6.2449979983983903</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>6.24499799839839</c:v>
+                  <c:v>6.2449979983983903</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>6.557438524302</c:v>
+                  <c:v>6.5574385243020004</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>6.08276253029821</c:v>
+                  <c:v>6.0827625302982096</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>6.32455532033675</c:v>
+                  <c:v>6.3245553203367502</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>6.16441400296897</c:v>
+                  <c:v>6.1644140029689698</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>7.07106781186547</c:v>
+                  <c:v>7.0710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>7.28010988928051</c:v>
+                  <c:v>7.2801098892805101</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>6.9282032302755</c:v>
+                  <c:v>6.9282032302754999</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>7.07106781186547</c:v>
+                  <c:v>7.0710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>7.14142842854285</c:v>
+                  <c:v>7.1414284285428504</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>7.07106781186547</c:v>
+                  <c:v>7.0710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>7.07106781186547</c:v>
+                  <c:v>7.0710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>9.48683298050513</c:v>
+                  <c:v>9.4868329805051292</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>9.53939201416945</c:v>
+                  <c:v>9.5393920141694508</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>9.32737905308881</c:v>
+                  <c:v>9.3273790530888103</c:v>
                 </c:pt>
                 <c:pt idx="197">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>9.32737905308881</c:v>
+                  <c:v>9.3273790530888103</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>9.2736184954957</c:v>
+                  <c:v>9.2736184954957004</c:v>
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>9.38083151964686</c:v>
+                  <c:v>9.3808315196468612</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>8.944271909999156</c:v>
+                  <c:v>8.9442719099991557</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>9.591663046625428</c:v>
+                  <c:v>9.5916630466254276</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>9.32737905308881</c:v>
+                  <c:v>9.3273790530888103</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>9.38083151964686</c:v>
+                  <c:v>9.3808315196468612</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="220">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>8.944271909999156</c:v>
+                  <c:v>8.9442719099991557</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791443027</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>7.34846922834953</c:v>
+                  <c:v>7.3484692283495301</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>7.87400787401181</c:v>
+                  <c:v>7.8740078740118102</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>7.6157731058639</c:v>
+                  <c:v>7.6157731058638998</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>7.28010988928051</c:v>
+                  <c:v>7.2801098892805101</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>7.21110255092797</c:v>
+                  <c:v>7.2111025509279703</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>7.87400787401181</c:v>
+                  <c:v>7.8740078740118102</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>7.87400787401181</c:v>
+                  <c:v>7.8740078740118102</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="244">
                   <c:v>7.48331477354788</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>7.41619848709566</c:v>
+                  <c:v>7.4161984870956603</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>7.6157731058639</c:v>
+                  <c:v>7.6157731058638998</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>8.124038404635961</c:v>
+                  <c:v>8.1240384046359608</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="280">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="281">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="282">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="283">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="284">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="285">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="286">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="287">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="288">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="289">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="290">
-                  <c:v>7.6811457478686</c:v>
+                  <c:v>7.6811457478685998</c:v>
                 </c:pt>
                 <c:pt idx="291">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="294">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="295">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="296">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="298">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="299">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="300">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="301">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="302">
-                  <c:v>8.124038404635961</c:v>
+                  <c:v>8.1240384046359608</c:v>
                 </c:pt>
                 <c:pt idx="303">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="304">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="305">
-                  <c:v>8.124038404635961</c:v>
+                  <c:v>8.1240384046359608</c:v>
                 </c:pt>
                 <c:pt idx="306">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="307">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="308">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="309">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="310">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="311">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="312">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="313">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="314">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="315">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="316">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="317">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="318">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="319">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="320">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="321">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="322">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="323">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="324">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="326">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="327">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="328">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="329">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="330">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="331">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="332">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="333">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="334">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791442992</c:v>
                 </c:pt>
                 <c:pt idx="335">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="336">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="337">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="338">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="339">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="340">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="341">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="342">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="343">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="344">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="345">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="346">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="347">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="348">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="349">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="350">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="351">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="352">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="353">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="354">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="355">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="356">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="357">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="358">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="359">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="360">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="361">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="362">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="363">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="364">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="365">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="366">
-                  <c:v>7.6157731058639</c:v>
+                  <c:v>7.6157731058638998</c:v>
                 </c:pt>
                 <c:pt idx="367">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="368">
-                  <c:v>7.54983443527075</c:v>
+                  <c:v>7.5498344352707498</c:v>
                 </c:pt>
                 <c:pt idx="369">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="370">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="371">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="372">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="373">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="374">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="375">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="376">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="377">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="378">
-                  <c:v>8.124038404635961</c:v>
+                  <c:v>8.1240384046359608</c:v>
                 </c:pt>
                 <c:pt idx="379">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="380">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="381">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="382">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="383">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="384">
-                  <c:v>9.1104335791443</c:v>
+                  <c:v>9.1104335791442992</c:v>
                 </c:pt>
                 <c:pt idx="385">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="386">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="387">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="388">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="389">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="390">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="391">
-                  <c:v>7.87400787401181</c:v>
+                  <c:v>7.8740078740118102</c:v>
                 </c:pt>
                 <c:pt idx="392">
-                  <c:v>8.774964387392121</c:v>
+                  <c:v>8.7749643873921208</c:v>
                 </c:pt>
                 <c:pt idx="393">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="394">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="395">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="396">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="397">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="398">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="399">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="400">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="401">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="402">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="403">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="404">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="405">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="406">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="407">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="408">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="409">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="410">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="411">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="412">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="413">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="414">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="415">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="416">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="417">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="418">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="419">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="420">
-                  <c:v>9.05538513813741</c:v>
+                  <c:v>9.0553851381374102</c:v>
                 </c:pt>
                 <c:pt idx="421">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="422">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="423">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="424">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="425">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="426">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="427">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="428">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="429">
-                  <c:v>7.93725393319377</c:v>
+                  <c:v>7.9372539331937704</c:v>
                 </c:pt>
                 <c:pt idx="430">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="431">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="432">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="433">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="434">
-                  <c:v>8.30662386291807</c:v>
+                  <c:v>8.3066238629180695</c:v>
                 </c:pt>
                 <c:pt idx="435">
-                  <c:v>9.16515138991168</c:v>
+                  <c:v>9.1651513899116797</c:v>
                 </c:pt>
                 <c:pt idx="436">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="437">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="438">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="439">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="440">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="441">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="442">
-                  <c:v>8.83176086632784</c:v>
+                  <c:v>8.8317608663278406</c:v>
                 </c:pt>
                 <c:pt idx="443">
-                  <c:v>8.944271909999159</c:v>
+                  <c:v>8.9442719099991592</c:v>
                 </c:pt>
                 <c:pt idx="444">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="445">
-                  <c:v>8.88819441731558</c:v>
+                  <c:v>8.8881944173155798</c:v>
                 </c:pt>
                 <c:pt idx="446">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="447">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="448">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="449">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="450">
-                  <c:v>8.54400374531753</c:v>
+                  <c:v>8.5440037453175304</c:v>
                 </c:pt>
                 <c:pt idx="451">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="452">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="453">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="454">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="455">
-                  <c:v>8.18535277187245</c:v>
+                  <c:v>8.1853527718724504</c:v>
                 </c:pt>
                 <c:pt idx="456">
-                  <c:v>9.2736184954957</c:v>
+                  <c:v>9.2736184954957004</c:v>
                 </c:pt>
                 <c:pt idx="457">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="458">
                   <c:v>9.21954445729288</c:v>
                 </c:pt>
                 <c:pt idx="459">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="460">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="461">
-                  <c:v>8.246211251235319</c:v>
+                  <c:v>8.2462112512353194</c:v>
                 </c:pt>
                 <c:pt idx="462">
-                  <c:v>8.06225774829855</c:v>
+                  <c:v>8.0622577482985491</c:v>
                 </c:pt>
                 <c:pt idx="463">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="464">
-                  <c:v>8.71779788708134</c:v>
+                  <c:v>8.7177978870813408</c:v>
                 </c:pt>
                 <c:pt idx="465">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="466">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="467">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="468">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="469">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>8.4852813742385695</c:v>
                 </c:pt>
                 <c:pt idx="470">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="471">
-                  <c:v>7.81024967590665</c:v>
+                  <c:v>7.8102496759066504</c:v>
                 </c:pt>
                 <c:pt idx="472">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="473">
-                  <c:v>7.74596669241483</c:v>
+                  <c:v>7.7459666924148296</c:v>
                 </c:pt>
                 <c:pt idx="474">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
                 <c:pt idx="475">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="476">
-                  <c:v>8.36660026534075</c:v>
+                  <c:v>8.3666002653407503</c:v>
                 </c:pt>
                 <c:pt idx="477">
-                  <c:v>8.42614977317635</c:v>
+                  <c:v>8.4261497731763502</c:v>
                 </c:pt>
                 <c:pt idx="478">
-                  <c:v>8.60232526704262</c:v>
+                  <c:v>8.6023252670426196</c:v>
                 </c:pt>
                 <c:pt idx="479">
-                  <c:v>8.66025403784438</c:v>
+                  <c:v>8.6602540378443802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="473545672"/>
-        <c:axId val="473548776"/>
+        <c:axId val="89765376"/>
+        <c:axId val="149781120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="473545672"/>
+        <c:axId val="89765376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Size, m</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="473548776"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149781120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="473548776"/>
+        <c:axId val="149781120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15.0"/>
+          <c:max val="15"/>
         </c:scaling>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Standard</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Deviation in Attendance of Choice A</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="473545672"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89765376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.0"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -3024,7 +3099,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -3377,14 +3452,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B480"/>
   <sheetViews>
     <sheetView topLeftCell="A452" workbookViewId="0">
       <selection activeCell="A481" sqref="A481:XFD481"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">

</xml_diff>